<commit_message>
done display voicedline, and fixed linelog issues
</commit_message>
<xml_diff>
--- a/Script Format Reference.xlsx
+++ b/Script Format Reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cai_y\Desktop\Visual Novel Engine\SFML_tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF3C9563-FCC7-4254-A0B1-14D302F67B61}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59660C5-9F4F-4D18-8BA5-BBC210D550DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24045" yWindow="345" windowWidth="21600" windowHeight="11385" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="103">
   <si>
     <t>Line</t>
   </si>
@@ -326,6 +326,21 @@
   </si>
   <si>
     <t>None/Wait</t>
+  </si>
+  <si>
+    <t>[Voice2(optional)]</t>
+  </si>
+  <si>
+    <t>[Voice3(optional)]</t>
+  </si>
+  <si>
+    <t>VoicedLine (or vl, voice, v)</t>
+  </si>
+  <si>
+    <t>[Voice, note that you need to specify full path from "sound/" folder]</t>
+  </si>
+  <si>
+    <t>None (Instant behavior is undefined)</t>
   </si>
 </sst>
 </file>
@@ -738,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AF088D-1F36-4E3F-BFB9-CD97E17BC052}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,10 +764,12 @@
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.42578125" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="63" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1072,67 +1089,82 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>46</v>
+      <c r="B18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1143,127 +1175,133 @@
         <v>50</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>53</v>
@@ -1271,27 +1309,24 @@
       <c r="C37" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>53</v>
@@ -1303,23 +1338,23 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>93</v>
+    <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>37</v>
+        <v>95</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>96</v>
@@ -1328,6 +1363,20 @@
         <v>97</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>93</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed save/load, note that you need to remove all saved files
</commit_message>
<xml_diff>
--- a/Script Format Reference.xlsx
+++ b/Script Format Reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cai_y\Desktop\Visual Novel Engine\SFML_tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59660C5-9F4F-4D18-8BA5-BBC210D550DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD21E80-B4BB-4680-944F-E5019011F64F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AF088D-1F36-4E3F-BFB9-CD97E17BC052}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,35 +1089,35 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" s="1" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
done with loop-related commands
</commit_message>
<xml_diff>
--- a/Script Format Reference.xlsx
+++ b/Script Format Reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cai_y\Desktop\Visual Novel Engine\SFML_tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD21E80-B4BB-4680-944F-E5019011F64F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CEB6B9-1E9A-47E7-ACC4-1B703C44E616}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="105">
   <si>
     <t>Line</t>
   </si>
@@ -142,15 +142,9 @@
     <t>Jump</t>
   </si>
   <si>
-    <t>Script</t>
-  </si>
-  <si>
     <t>End</t>
   </si>
   <si>
-    <t>None/Exclaimation/Gorey/Instant?</t>
-  </si>
-  <si>
     <t>Hide</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>Delay</t>
   </si>
   <si>
-    <t>Append</t>
-  </si>
-  <si>
     <t>flag2</t>
   </si>
   <si>
@@ -199,12 +190,6 @@
     <t>EndLoop</t>
   </si>
   <si>
-    <t>Commands</t>
-  </si>
-  <si>
-    <t>numLoop("infinite" for endless loop)</t>
-  </si>
-  <si>
     <t>Loopname</t>
   </si>
   <si>
@@ -307,12 +292,6 @@
     <t>gradual? Relative?</t>
   </si>
   <si>
-    <t>start_blur</t>
-  </si>
-  <si>
-    <t>end_blur</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
@@ -341,6 +320,33 @@
   </si>
   <si>
     <t>None (Instant behavior is undefined)</t>
+  </si>
+  <si>
+    <t>[number of loops ("infinite" for endless loop, 1 by default)]</t>
+  </si>
+  <si>
+    <t>[blur_radius (0 to 1)]</t>
+  </si>
+  <si>
+    <t>[time]</t>
+  </si>
+  <si>
+    <t>#NOTE: This is used to signify where the scope of the loop ends</t>
+  </si>
+  <si>
+    <t>#NOTE: this is meant to be used after EndLoop, to manually stop the loop forcefully (necessary for stopping infinite loop)</t>
+  </si>
+  <si>
+    <t>#NOTE: this is meant to be used before EndLoop, to manually stop the loop from within the loop</t>
+  </si>
+  <si>
+    <t>#NOTE: this is meant to be used before EndLoop, to jump to the beginning of the loop and increment the loop counter by 1. Executing commands will NOT  stop</t>
+  </si>
+  <si>
+    <t>ClearLoop</t>
+  </si>
+  <si>
+    <t>#NOTE: this is meant to clear all commands in the execution queue, regardless of whether or not they are finished executing</t>
   </si>
 </sst>
 </file>
@@ -753,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AF088D-1F36-4E3F-BFB9-CD97E17BC052}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,8 +770,8 @@
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="63" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
@@ -816,19 +822,19 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -842,19 +848,19 @@
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -865,28 +871,28 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -897,28 +903,28 @@
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -929,22 +935,22 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -958,10 +964,10 @@
         <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -975,27 +981,27 @@
         <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1009,16 +1015,16 @@
         <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1026,13 +1032,13 @@
         <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1040,30 +1046,30 @@
         <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1074,19 +1080,19 @@
         <v>0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1094,31 +1100,31 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1138,19 +1144,19 @@
         <v>26</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1164,7 +1170,7 @@
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1172,16 +1178,16 @@
         <v>35</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1189,52 +1195,52 @@
         <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>10</v>
@@ -1243,141 +1249,148 @@
         <v>24</v>
       </c>
       <c r="D28" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="B36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="B40" s="2" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added start and end cinematic bars command
</commit_message>
<xml_diff>
--- a/Script Format Reference.xlsx
+++ b/Script Format Reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cai_y\Desktop\Visual Novel Engine\SFML_tester\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CEB6B9-1E9A-47E7-ACC4-1B703C44E616}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6104E6C7-3C21-43C1-A679-5ECD82461A86}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{728A89CD-FEF5-4E0A-92F7-C7008FCA604F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="106">
   <si>
     <t>Line</t>
   </si>
@@ -292,9 +292,6 @@
     <t>gradual? Relative?</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
     <t>flag1 (use comma (,) to separate mutliple flags)</t>
   </si>
   <si>
@@ -347,13 +344,19 @@
   </si>
   <si>
     <t>#NOTE: this is meant to clear all commands in the execution queue, regardless of whether or not they are finished executing</t>
+  </si>
+  <si>
+    <t>[time=1]</t>
+  </si>
+  <si>
+    <t>[Height=100]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,13 +372,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
@@ -384,7 +380,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,11 +390,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -431,21 +422,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
+  <cellStyles count="3">
+    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -761,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AF088D-1F36-4E3F-BFB9-CD97E17BC052}">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,35 +766,35 @@
     <col min="10" max="10" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -998,10 +986,10 @@
         <v>66</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1100,10 +1088,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>66</v>
@@ -1112,19 +1100,19 @@
         <v>70</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>71</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>72</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1144,7 +1132,7 @@
         <v>26</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>27</v>
@@ -1280,7 +1268,7 @@
         <v>52</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1291,7 +1279,7 @@
         <v>50</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1311,7 +1299,7 @@
         <v>83</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1328,7 +1316,7 @@
         <v>83</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1345,12 +1333,12 @@
         <v>83</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>50</v>
@@ -1362,35 +1350,38 @@
         <v>83</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="E39" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>86</v>
+      <c r="D40" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>